<commit_message>
DEV1.2 - Project Management
</commit_message>
<xml_diff>
--- a/resources/data/ProjectList.xlsx
+++ b/resources/data/ProjectList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
   <si>
     <t>Project Name</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>Hidden</t>
+  </si>
+  <si>
+    <t>Savannah Condopark</t>
+  </si>
+  <si>
+    <t>Simei</t>
+  </si>
+  <si>
+    <t>Visible</t>
   </si>
 </sst>
 </file>
@@ -1048,15 +1057,15 @@
         <v>24</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -1088,11 +1097,8 @@
       <c r="L3" t="n">
         <v>3.0</v>
       </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
       <c r="N3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DEV1.3 - Project Management
</commit_message>
<xml_diff>
--- a/resources/data/ProjectList.xlsx
+++ b/resources/data/ProjectList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a02774ed8d28bca/Desktop/NTU/NTU_Y1S2/SC2002/Assignment/BTO_Application/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racshanyaa/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74E5F81C-5936-4553-AEBF-6910ECA9F620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27341D7D-F181-284D-9371-FA1DC913DE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="11100" windowHeight="11768" xr2:uid="{EC828834-49F0-4F3D-9E02-12D77198102E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" xr2:uid="{EC828834-49F0-4F3D-9E02-12D77198102E}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectList" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>Project Name</t>
   </si>
@@ -67,24 +67,6 @@
     <t>Yishun</t>
   </si>
   <si>
-    <t>2-Room</t>
-  </si>
-  <si>
-    <t>3-Room</t>
-  </si>
-  <si>
-    <t>Jessica</t>
-  </si>
-  <si>
-    <t>Daniel,Emily</t>
-  </si>
-  <si>
-    <t>savannah</t>
-  </si>
-  <si>
-    <t>simei</t>
-  </si>
-  <si>
     <t>2-ROOM</t>
   </si>
   <si>
@@ -97,16 +79,28 @@
     <t>N/A</t>
   </si>
   <si>
+    <t>Savannah Condopark</t>
+  </si>
+  <si>
+    <t>Simei</t>
+  </si>
+  <si>
+    <t>Visible</t>
+  </si>
+  <si>
+    <t>Project ID</t>
+  </si>
+  <si>
+    <t>Tampines</t>
+  </si>
+  <si>
+    <t>Melvill Park</t>
+  </si>
+  <si>
+    <t>Melville Park</t>
+  </si>
+  <si>
     <t>Hidden</t>
-  </si>
-  <si>
-    <t>Savannah Condopark</t>
-  </si>
-  <si>
-    <t>Simei</t>
-  </si>
-  <si>
-    <t>Visible</t>
   </si>
 </sst>
 </file>
@@ -591,9 +585,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -969,136 +962,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{335DBED5-A3D5-4E35-8BEF-221CF426CB16}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>350000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>450000</v>
+      </c>
+      <c r="J2">
+        <v>45703</v>
+      </c>
+      <c r="K2">
+        <v>45736</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>350000.0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="n">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>100000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>100000</v>
+      </c>
+      <c r="J3">
+        <v>45775</v>
+      </c>
+      <c r="K3">
+        <v>45805</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>3.0</v>
       </c>
-      <c r="H2" t="n">
-        <v>450000.0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>45703.0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>45736.0</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1000000.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2000000.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>45775.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>45805.0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="O4" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>100000.0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>100000.0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>45775.0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>45805.0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DEV 10 - Bug Fix to Manager Project
</commit_message>
<xml_diff>
--- a/resources/data/ProjectList.xlsx
+++ b/resources/data/ProjectList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="38">
   <si>
     <t>Project Name</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Flora Dr</t>
+  </si>
+  <si>
+    <t>Michael</t>
   </si>
 </sst>
 </file>
@@ -992,7 +995,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{335DBED5-A3D5-4E35-8BEF-221CF426CB16}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
@@ -1085,7 +1088,7 @@
         <v>45805.0</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="M2" t="n">
         <v>5.0</v>
@@ -1229,50 +1232,6 @@
         <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1000000.0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>2000000.0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>45775.0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>45805.0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="O6" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>